<commit_message>
Set up KPO4 over time graph to show bar graph if only 1 quarter of data is available. Added extra quarter to dummy data to test
</commit_message>
<xml_diff>
--- a/DummyData_3.xlsx
+++ b/DummyData_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\building-standards-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C9D98AA-658C-44A8-B936-152BEAE92E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D9CEFE-528E-40B7-9616-8054F04C875A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="132">
   <si>
     <t>UserID</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>11:18:43.293</t>
+  </si>
+  <si>
+    <t>2021-12-25</t>
   </si>
 </sst>
 </file>
@@ -452,8 +455,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,13 +772,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN13"/>
+  <dimension ref="A1:CN15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CN1" sqref="CN1"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:92">
       <c r="A1" t="s">
@@ -4243,6 +4251,538 @@
         <v>76</v>
       </c>
       <c r="CN13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:92">
+      <c r="A14">
+        <v>187370435</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>71</v>
+      </c>
+      <c r="U14" t="s">
+        <v>76</v>
+      </c>
+      <c r="V14" t="s">
+        <v>71</v>
+      </c>
+      <c r="W14" t="s">
+        <v>77</v>
+      </c>
+      <c r="X14" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BP14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BR14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BT14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BV14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BW14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BX14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BY14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CB14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CC14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CF14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CG14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CH14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CI14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CJ14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CK14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CL14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM14" t="s">
+        <v>76</v>
+      </c>
+      <c r="CN14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:92">
+      <c r="A15">
+        <v>187370436</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>113</v>
+      </c>
+      <c r="U15" t="s">
+        <v>76</v>
+      </c>
+      <c r="V15" t="s">
+        <v>76</v>
+      </c>
+      <c r="W15" t="s">
+        <v>76</v>
+      </c>
+      <c r="X15" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM15">
+        <v>1</v>
+      </c>
+      <c r="AN15">
+        <v>2</v>
+      </c>
+      <c r="AO15">
+        <v>3</v>
+      </c>
+      <c r="AP15">
+        <v>4</v>
+      </c>
+      <c r="AQ15">
+        <v>5</v>
+      </c>
+      <c r="AR15">
+        <v>4</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>77</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>76</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BA15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BP15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BQ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BR15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BT15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BU15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BV15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BW15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BX15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BY15" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CC15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CD15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CF15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CG15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CH15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CI15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CJ15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CK15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CL15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CM15" t="s">
+        <v>76</v>
+      </c>
+      <c r="CN15" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>